<commit_message>
fixes to pass validation against xsd
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -91,7 +91,7 @@
     <t>HEBACY2N</t>
   </si>
   <si>
-    <t>CYXX XXXX XXXX XXXX XXXX XXXX XXXX</t>
+    <t>CY12 1234 4321 1234 4321 1234 4321</t>
   </si>
   <si>
     <t>€</t>
@@ -103,19 +103,19 @@
     <t>BCYPCY2N</t>
   </si>
   <si>
-    <t>CYXX XXXX YYYY ZZZZ XXXX YYYY ZZZZ</t>
+    <t>CY11 3333 2222 2222 2222 4444 3332</t>
   </si>
   <si>
     <t>RICH LTD</t>
   </si>
   <si>
-    <t>CYPP YYYY ZZZZ XXXX YYYY ZZZZ XXXX</t>
+    <t>CY33 1111 2222 2222 2222 2222 2222</t>
   </si>
   <si>
     <t>BONOBO ELECTRONICS</t>
   </si>
   <si>
-    <t>CYWW CCCC YYYY 0000 PPPP XXXX KKKK</t>
+    <t>CY45 3333 3333 0000 3333 3333 3333</t>
   </si>
   <si>
     <t>SOMETHING  ITALIA</t>
@@ -124,7 +124,7 @@
     <t>BANCA2</t>
   </si>
   <si>
-    <t>ITPP YYYY ZZZZ IIII YYYY LLLL AAAA</t>
+    <t>IT44 5555 5555 5555 5555 5555 5555</t>
   </si>
   <si>
     <t>Totals:</t>

</xml_diff>